<commit_message>
Attempt output several graphics to screen. Test_0
</commit_message>
<xml_diff>
--- a/t_12/TouchGFX/assets/texts/texts.xlsx
+++ b/t_12/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="83">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -233,6 +233,39 @@
   </si>
   <si>
     <t xml:space="preserve">Value: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-., 0123456789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId10</t>
   </si>
 </sst>
 </file>
@@ -1480,7 +1513,9 @@
         <v>48</v>
       </c>
       <c r="I4"/>
-      <c r="J4"/>
+      <c r="J4" t="s">
+        <v>72</v>
+      </c>
       <c r="K4" s="5" t="s">
         <v>17</v>
       </c>
@@ -1747,12 +1782,142 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="2:10"/>
-    <row r="8" spans="2:10"/>
-    <row r="9" spans="2:10"/>
-    <row r="10" spans="2:10"/>
-    <row r="13" spans="2:10"/>
-    <row r="14" spans="2:10"/>
+    <row r="7" spans="2:10">
+      <c r="B7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="15" spans="2:10"/>
     <row r="16" spans="2:10"/>
     <row r="17" spans="4:4"/>

</xml_diff>

<commit_message>
#1 Added labels to graphic
</commit_message>
<xml_diff>
--- a/t_12/TouchGFX/assets/texts/texts.xlsx
+++ b/t_12/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="90">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -266,6 +266,27 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;currXValue&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;currYValue&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TextId2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TextId3</t>
   </si>
 </sst>
 </file>
@@ -1540,7 +1561,7 @@
         <v>69</v>
       </c>
       <c r="D5">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -1553,7 +1574,9 @@
         <v>48</v>
       </c>
       <c r="I5"/>
-      <c r="J5"/>
+      <c r="J5" t="s">
+        <v>72</v>
+      </c>
       <c r="K5" s="8" t="s">
         <v>1</v>
       </c>
@@ -1569,7 +1592,27 @@
       <c r="O5" s="11"/>
     </row>
     <row r="6" spans="2:15">
+      <c r="B6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6"/>
+      <c r="H6" t="s">
+        <v>48</v>
+      </c>
       <c r="I6"/>
+      <c r="J6"/>
       <c r="K6" s="8" t="s">
         <v>2</v>
       </c>
@@ -1770,7 +1813,7 @@
         <v>65</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="D6" t="s">
         <v>62</v>
@@ -1818,16 +1861,16 @@
     </row>
     <row r="9" spans="2:10">
       <c r="B9" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="F9" t="s">
         <v>59</v>
@@ -1835,89 +1878,25 @@
     </row>
     <row r="10" spans="2:10">
       <c r="B10" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="F10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11">
-      <c r="B11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" t="s">
-        <v>74</v>
-      </c>
-      <c r="F11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" t="s">
-        <v>80</v>
-      </c>
-      <c r="C12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" t="s">
-        <v>74</v>
-      </c>
-      <c r="F12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10">
-      <c r="B13" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" t="s">
-        <v>74</v>
-      </c>
-      <c r="F13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10">
-      <c r="B14" t="s">
-        <v>82</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" t="s">
-        <v>74</v>
-      </c>
-      <c r="F14" t="s">
-        <v>59</v>
-      </c>
-    </row>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13" spans="2:10"/>
+    <row r="14" spans="2:10"/>
     <row r="15" spans="2:10"/>
     <row r="16" spans="2:10"/>
     <row r="17" spans="4:4"/>

</xml_diff>

<commit_message>
Change russian text to svg_0
</commit_message>
<xml_diff>
--- a/t_12/TouchGFX/assets/texts/texts.xlsx
+++ b/t_12/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8249" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9197" uniqueCount="199">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2241,16 +2241,16 @@
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="D11" t="s">
         <v>62</v>
       </c>
       <c r="E11" t="s">
-        <v>118</v>
+        <v>46</v>
       </c>
       <c r="F11" t="s">
         <v>59</v>
@@ -2258,7 +2258,7 @@
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C12" t="s">
         <v>88</v>
@@ -2275,7 +2275,7 @@
     </row>
     <row r="13" spans="2:10">
       <c r="B13" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C13" t="s">
         <v>88</v>
@@ -2284,7 +2284,7 @@
         <v>62</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>121</v>
       </c>
       <c r="F13" t="s">
         <v>59</v>
@@ -2292,7 +2292,7 @@
     </row>
     <row r="14" spans="2:10">
       <c r="B14" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C14" t="s">
         <v>88</v>
@@ -2309,7 +2309,7 @@
     </row>
     <row r="15" spans="2:10">
       <c r="B15" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C15" t="s">
         <v>88</v>
@@ -2318,7 +2318,7 @@
         <v>62</v>
       </c>
       <c r="E15" t="s">
-        <v>120</v>
+        <v>46</v>
       </c>
       <c r="F15" t="s">
         <v>59</v>
@@ -2326,7 +2326,7 @@
     </row>
     <row r="16" spans="2:10">
       <c r="B16" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C16" t="s">
         <v>88</v>
@@ -2335,7 +2335,7 @@
         <v>62</v>
       </c>
       <c r="E16" t="s">
-        <v>121</v>
+        <v>166</v>
       </c>
       <c r="F16" t="s">
         <v>59</v>
@@ -2343,7 +2343,7 @@
     </row>
     <row r="17" spans="4:4">
       <c r="B17" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="C17" t="s">
         <v>88</v>
@@ -2360,7 +2360,7 @@
     </row>
     <row r="18" spans="4:4">
       <c r="B18" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
       <c r="C18" t="s">
         <v>88</v>
@@ -2377,7 +2377,7 @@
     </row>
     <row r="19" spans="4:4">
       <c r="B19" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="C19" t="s">
         <v>88</v>
@@ -2386,7 +2386,7 @@
         <v>62</v>
       </c>
       <c r="E19" t="s">
-        <v>162</v>
+        <v>46</v>
       </c>
       <c r="F19" t="s">
         <v>59</v>
@@ -2394,16 +2394,16 @@
     </row>
     <row r="20" spans="4:4">
       <c r="B20" t="s">
-        <v>130</v>
+        <v>151</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="D20" t="s">
         <v>62</v>
       </c>
       <c r="E20" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="F20" t="s">
         <v>59</v>
@@ -2411,7 +2411,7 @@
     </row>
     <row r="21" spans="4:4">
       <c r="B21" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="C21" t="s">
         <v>88</v>
@@ -2420,7 +2420,7 @@
         <v>62</v>
       </c>
       <c r="E21" t="s">
-        <v>164</v>
+        <v>46</v>
       </c>
       <c r="F21" t="s">
         <v>59</v>
@@ -2428,7 +2428,7 @@
     </row>
     <row r="22" spans="4:4">
       <c r="B22" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C22" t="s">
         <v>88</v>
@@ -2437,7 +2437,7 @@
         <v>62</v>
       </c>
       <c r="E22" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F22" t="s">
         <v>59</v>
@@ -2445,7 +2445,7 @@
     </row>
     <row r="23" spans="4:4">
       <c r="B23" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="C23" t="s">
         <v>88</v>
@@ -2462,7 +2462,7 @@
     </row>
     <row r="24" spans="4:4">
       <c r="B24" t="s">
-        <v>149</v>
+        <v>168</v>
       </c>
       <c r="C24" t="s">
         <v>88</v>
@@ -2471,7 +2471,7 @@
         <v>62</v>
       </c>
       <c r="E24" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F24" t="s">
         <v>59</v>
@@ -2479,7 +2479,7 @@
     </row>
     <row r="25" spans="4:4">
       <c r="B25" t="s">
-        <v>150</v>
+        <v>169</v>
       </c>
       <c r="C25" t="s">
         <v>88</v>
@@ -2496,7 +2496,7 @@
     </row>
     <row r="26" spans="4:4">
       <c r="B26" t="s">
-        <v>151</v>
+        <v>170</v>
       </c>
       <c r="C26" t="s">
         <v>88</v>
@@ -2505,7 +2505,7 @@
         <v>62</v>
       </c>
       <c r="E26" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F26" t="s">
         <v>59</v>
@@ -2513,7 +2513,7 @@
     </row>
     <row r="27" spans="4:4">
       <c r="B27" t="s">
-        <v>152</v>
+        <v>171</v>
       </c>
       <c r="C27" t="s">
         <v>88</v>
@@ -2530,7 +2530,7 @@
     </row>
     <row r="28" spans="4:4">
       <c r="B28" t="s">
-        <v>153</v>
+        <v>172</v>
       </c>
       <c r="C28" t="s">
         <v>88</v>
@@ -2539,7 +2539,7 @@
         <v>62</v>
       </c>
       <c r="E28" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F28" t="s">
         <v>59</v>
@@ -2547,7 +2547,7 @@
     </row>
     <row r="29" spans="4:4">
       <c r="B29" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="C29" t="s">
         <v>88</v>
@@ -2564,7 +2564,7 @@
     </row>
     <row r="30" spans="4:4">
       <c r="B30" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="C30" t="s">
         <v>88</v>
@@ -2581,16 +2581,16 @@
     </row>
     <row r="31" spans="4:4">
       <c r="B31" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="C31" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="D31" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E31" t="s">
-        <v>46</v>
+        <v>177</v>
       </c>
       <c r="F31" t="s">
         <v>59</v>
@@ -2598,16 +2598,16 @@
     </row>
     <row r="32" spans="4:4">
       <c r="B32" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="C32" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="D32" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E32" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="F32" t="s">
         <v>59</v>
@@ -2615,7 +2615,7 @@
     </row>
     <row r="33" spans="4:4">
       <c r="B33" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="C33" t="s">
         <v>88</v>
@@ -2624,7 +2624,7 @@
         <v>62</v>
       </c>
       <c r="E33" t="s">
-        <v>46</v>
+        <v>180</v>
       </c>
       <c r="F33" t="s">
         <v>59</v>
@@ -2632,7 +2632,7 @@
     </row>
     <row r="34" spans="4:4">
       <c r="B34" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="C34" t="s">
         <v>88</v>
@@ -2641,7 +2641,7 @@
         <v>62</v>
       </c>
       <c r="E34" t="s">
-        <v>167</v>
+        <v>94</v>
       </c>
       <c r="F34" t="s">
         <v>59</v>
@@ -2649,7 +2649,7 @@
     </row>
     <row r="35" spans="4:4">
       <c r="B35" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="C35" t="s">
         <v>88</v>
@@ -2658,7 +2658,7 @@
         <v>62</v>
       </c>
       <c r="E35" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="F35" t="s">
         <v>59</v>
@@ -2666,7 +2666,7 @@
     </row>
     <row r="36" spans="4:4">
       <c r="B36" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="C36" t="s">
         <v>88</v>
@@ -2675,7 +2675,7 @@
         <v>62</v>
       </c>
       <c r="E36" t="s">
-        <v>167</v>
+        <v>94</v>
       </c>
       <c r="F36" t="s">
         <v>59</v>
@@ -2683,16 +2683,16 @@
     </row>
     <row r="37" spans="4:4">
       <c r="B37" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="C37" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="D37" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E37" t="s">
-        <v>177</v>
+        <v>63</v>
       </c>
       <c r="F37" t="s">
         <v>59</v>
@@ -2700,16 +2700,16 @@
     </row>
     <row r="38" spans="4:4">
       <c r="B38" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="C38" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="D38" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E38" t="s">
-        <v>177</v>
+        <v>94</v>
       </c>
       <c r="F38" t="s">
         <v>59</v>
@@ -2717,7 +2717,7 @@
     </row>
     <row r="39" spans="4:4">
       <c r="B39" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="C39" t="s">
         <v>88</v>
@@ -2726,7 +2726,7 @@
         <v>62</v>
       </c>
       <c r="E39" t="s">
-        <v>180</v>
+        <v>63</v>
       </c>
       <c r="F39" t="s">
         <v>59</v>
@@ -2734,7 +2734,7 @@
     </row>
     <row r="40" spans="4:4">
       <c r="B40" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="C40" t="s">
         <v>88</v>
@@ -2743,7 +2743,7 @@
         <v>62</v>
       </c>
       <c r="E40" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="F40" t="s">
         <v>59</v>
@@ -2751,7 +2751,7 @@
     </row>
     <row r="41" spans="4:4">
       <c r="B41" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="C41" t="s">
         <v>88</v>
@@ -2760,7 +2760,7 @@
         <v>62</v>
       </c>
       <c r="E41" t="s">
-        <v>63</v>
+        <v>180</v>
       </c>
       <c r="F41" t="s">
         <v>59</v>
@@ -2768,7 +2768,7 @@
     </row>
     <row r="42" spans="4:4">
       <c r="B42" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="C42" t="s">
         <v>88</v>
@@ -2777,7 +2777,7 @@
         <v>62</v>
       </c>
       <c r="E42" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="F42" t="s">
         <v>59</v>
@@ -2785,7 +2785,7 @@
     </row>
     <row r="43" spans="4:4">
       <c r="B43" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C43" t="s">
         <v>88</v>
@@ -2794,7 +2794,7 @@
         <v>62</v>
       </c>
       <c r="E43" t="s">
-        <v>63</v>
+        <v>180</v>
       </c>
       <c r="F43" t="s">
         <v>59</v>
@@ -2802,7 +2802,7 @@
     </row>
     <row r="44" spans="4:4">
       <c r="B44" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="C44" t="s">
         <v>88</v>
@@ -2811,7 +2811,7 @@
         <v>62</v>
       </c>
       <c r="E44" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="F44" t="s">
         <v>59</v>
@@ -2819,7 +2819,7 @@
     </row>
     <row r="45" spans="4:4">
       <c r="B45" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="C45" t="s">
         <v>88</v>
@@ -2828,7 +2828,7 @@
         <v>62</v>
       </c>
       <c r="E45" t="s">
-        <v>63</v>
+        <v>180</v>
       </c>
       <c r="F45" t="s">
         <v>59</v>
@@ -2836,7 +2836,7 @@
     </row>
     <row r="46" spans="4:4">
       <c r="B46" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="C46" t="s">
         <v>88</v>
@@ -2853,7 +2853,7 @@
     </row>
     <row r="47" spans="4:4">
       <c r="B47" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="C47" t="s">
         <v>88</v>
@@ -2870,7 +2870,7 @@
     </row>
     <row r="48" spans="4:4">
       <c r="B48" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="C48" t="s">
         <v>88</v>
@@ -2879,7 +2879,7 @@
         <v>62</v>
       </c>
       <c r="E48" t="s">
-        <v>74</v>
+        <v>196</v>
       </c>
       <c r="F48" t="s">
         <v>59</v>
@@ -2887,7 +2887,7 @@
     </row>
     <row r="49" spans="4:4">
       <c r="B49" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="C49" t="s">
         <v>88</v>
@@ -2896,114 +2896,18 @@
         <v>62</v>
       </c>
       <c r="E49" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="F49" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="4:4">
-      <c r="B50" t="s">
-        <v>191</v>
-      </c>
-      <c r="C50" t="s">
-        <v>88</v>
-      </c>
-      <c r="D50" t="s">
-        <v>62</v>
-      </c>
-      <c r="E50" t="s">
-        <v>74</v>
-      </c>
-      <c r="F50" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="51" spans="4:4">
-      <c r="B51" t="s">
-        <v>192</v>
-      </c>
-      <c r="C51" t="s">
-        <v>88</v>
-      </c>
-      <c r="D51" t="s">
-        <v>62</v>
-      </c>
-      <c r="E51" t="s">
-        <v>180</v>
-      </c>
-      <c r="F51" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="52" spans="4:4">
-      <c r="B52" t="s">
-        <v>193</v>
-      </c>
-      <c r="C52" t="s">
-        <v>88</v>
-      </c>
-      <c r="D52" t="s">
-        <v>62</v>
-      </c>
-      <c r="E52" t="s">
-        <v>74</v>
-      </c>
-      <c r="F52" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="53" spans="4:4">
-      <c r="B53" t="s">
-        <v>194</v>
-      </c>
-      <c r="C53" t="s">
-        <v>88</v>
-      </c>
-      <c r="D53" t="s">
-        <v>62</v>
-      </c>
-      <c r="E53" t="s">
-        <v>180</v>
-      </c>
-      <c r="F53" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="54" spans="4:4">
-      <c r="B54" t="s">
-        <v>195</v>
-      </c>
-      <c r="C54" t="s">
-        <v>88</v>
-      </c>
-      <c r="D54" t="s">
-        <v>62</v>
-      </c>
-      <c r="E54" t="s">
-        <v>196</v>
-      </c>
-      <c r="F54" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="55" spans="4:4">
-      <c r="B55" t="s">
-        <v>197</v>
-      </c>
-      <c r="C55" t="s">
-        <v>88</v>
-      </c>
-      <c r="D55" t="s">
-        <v>62</v>
-      </c>
-      <c r="E55" t="s">
-        <v>198</v>
-      </c>
-      <c r="F55" t="s">
-        <v>59</v>
-      </c>
-    </row>
+    <row r="50" spans="4:4"/>
+    <row r="51" spans="4:4"/>
+    <row r="52" spans="4:4"/>
+    <row r="53" spans="4:4"/>
+    <row r="54" spans="4:4"/>
+    <row r="55" spans="4:4"/>
     <row r="56" spans="4:4"/>
     <row r="57" spans="4:4"/>
     <row r="58" spans="4:4"/>

</xml_diff>

<commit_message>
Change russian text to svg_1
</commit_message>
<xml_diff>
--- a/t_12/TouchGFX/assets/texts/texts.xlsx
+++ b/t_12/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9197" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9935" uniqueCount="199">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2315,7 +2315,7 @@
         <v>88</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
         <v>46</v>
@@ -2349,7 +2349,7 @@
         <v>88</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
         <v>46</v>
@@ -2383,7 +2383,7 @@
         <v>88</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E19" t="s">
         <v>46</v>
@@ -2417,7 +2417,7 @@
         <v>88</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E21" t="s">
         <v>46</v>
@@ -2445,16 +2445,16 @@
     </row>
     <row r="23" spans="4:4">
       <c r="B23" t="s">
-        <v>157</v>
+        <v>176</v>
       </c>
       <c r="C23" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E23" t="s">
-        <v>46</v>
+        <v>177</v>
       </c>
       <c r="F23" t="s">
         <v>59</v>
@@ -2462,16 +2462,16 @@
     </row>
     <row r="24" spans="4:4">
       <c r="B24" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="C24" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="D24" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E24" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="F24" t="s">
         <v>59</v>
@@ -2479,7 +2479,7 @@
     </row>
     <row r="25" spans="4:4">
       <c r="B25" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="C25" t="s">
         <v>88</v>
@@ -2488,7 +2488,7 @@
         <v>62</v>
       </c>
       <c r="E25" t="s">
-        <v>46</v>
+        <v>180</v>
       </c>
       <c r="F25" t="s">
         <v>59</v>
@@ -2496,7 +2496,7 @@
     </row>
     <row r="26" spans="4:4">
       <c r="B26" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="C26" t="s">
         <v>88</v>
@@ -2505,7 +2505,7 @@
         <v>62</v>
       </c>
       <c r="E26" t="s">
-        <v>167</v>
+        <v>94</v>
       </c>
       <c r="F26" t="s">
         <v>59</v>
@@ -2513,7 +2513,7 @@
     </row>
     <row r="27" spans="4:4">
       <c r="B27" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="C27" t="s">
         <v>88</v>
@@ -2522,7 +2522,7 @@
         <v>62</v>
       </c>
       <c r="E27" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="F27" t="s">
         <v>59</v>
@@ -2530,7 +2530,7 @@
     </row>
     <row r="28" spans="4:4">
       <c r="B28" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="C28" t="s">
         <v>88</v>
@@ -2539,7 +2539,7 @@
         <v>62</v>
       </c>
       <c r="E28" t="s">
-        <v>167</v>
+        <v>94</v>
       </c>
       <c r="F28" t="s">
         <v>59</v>
@@ -2547,7 +2547,7 @@
     </row>
     <row r="29" spans="4:4">
       <c r="B29" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="C29" t="s">
         <v>88</v>
@@ -2556,7 +2556,7 @@
         <v>62</v>
       </c>
       <c r="E29" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="F29" t="s">
         <v>59</v>
@@ -2564,7 +2564,7 @@
     </row>
     <row r="30" spans="4:4">
       <c r="B30" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="C30" t="s">
         <v>88</v>
@@ -2573,7 +2573,7 @@
         <v>62</v>
       </c>
       <c r="E30" t="s">
-        <v>167</v>
+        <v>94</v>
       </c>
       <c r="F30" t="s">
         <v>59</v>
@@ -2581,16 +2581,16 @@
     </row>
     <row r="31" spans="4:4">
       <c r="B31" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="D31" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E31" t="s">
-        <v>177</v>
+        <v>63</v>
       </c>
       <c r="F31" t="s">
         <v>59</v>
@@ -2598,16 +2598,16 @@
     </row>
     <row r="32" spans="4:4">
       <c r="B32" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="C32" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="D32" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E32" t="s">
-        <v>177</v>
+        <v>74</v>
       </c>
       <c r="F32" t="s">
         <v>59</v>
@@ -2615,7 +2615,7 @@
     </row>
     <row r="33" spans="4:4">
       <c r="B33" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="C33" t="s">
         <v>88</v>
@@ -2632,7 +2632,7 @@
     </row>
     <row r="34" spans="4:4">
       <c r="B34" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="C34" t="s">
         <v>88</v>
@@ -2641,7 +2641,7 @@
         <v>62</v>
       </c>
       <c r="E34" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="F34" t="s">
         <v>59</v>
@@ -2649,7 +2649,7 @@
     </row>
     <row r="35" spans="4:4">
       <c r="B35" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="C35" t="s">
         <v>88</v>
@@ -2658,7 +2658,7 @@
         <v>62</v>
       </c>
       <c r="E35" t="s">
-        <v>63</v>
+        <v>180</v>
       </c>
       <c r="F35" t="s">
         <v>59</v>
@@ -2666,7 +2666,7 @@
     </row>
     <row r="36" spans="4:4">
       <c r="B36" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="C36" t="s">
         <v>88</v>
@@ -2675,7 +2675,7 @@
         <v>62</v>
       </c>
       <c r="E36" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="F36" t="s">
         <v>59</v>
@@ -2683,7 +2683,7 @@
     </row>
     <row r="37" spans="4:4">
       <c r="B37" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="C37" t="s">
         <v>88</v>
@@ -2692,7 +2692,7 @@
         <v>62</v>
       </c>
       <c r="E37" t="s">
-        <v>63</v>
+        <v>180</v>
       </c>
       <c r="F37" t="s">
         <v>59</v>
@@ -2700,7 +2700,7 @@
     </row>
     <row r="38" spans="4:4">
       <c r="B38" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="C38" t="s">
         <v>88</v>
@@ -2709,7 +2709,7 @@
         <v>62</v>
       </c>
       <c r="E38" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="F38" t="s">
         <v>59</v>
@@ -2717,7 +2717,7 @@
     </row>
     <row r="39" spans="4:4">
       <c r="B39" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="C39" t="s">
         <v>88</v>
@@ -2726,182 +2726,22 @@
         <v>62</v>
       </c>
       <c r="E39" t="s">
-        <v>63</v>
+        <v>180</v>
       </c>
       <c r="F39" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="4:4">
-      <c r="B40" t="s">
-        <v>187</v>
-      </c>
-      <c r="C40" t="s">
-        <v>88</v>
-      </c>
-      <c r="D40" t="s">
-        <v>62</v>
-      </c>
-      <c r="E40" t="s">
-        <v>74</v>
-      </c>
-      <c r="F40" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="4:4">
-      <c r="B41" t="s">
-        <v>188</v>
-      </c>
-      <c r="C41" t="s">
-        <v>88</v>
-      </c>
-      <c r="D41" t="s">
-        <v>62</v>
-      </c>
-      <c r="E41" t="s">
-        <v>180</v>
-      </c>
-      <c r="F41" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="42" spans="4:4">
-      <c r="B42" t="s">
-        <v>189</v>
-      </c>
-      <c r="C42" t="s">
-        <v>88</v>
-      </c>
-      <c r="D42" t="s">
-        <v>62</v>
-      </c>
-      <c r="E42" t="s">
-        <v>74</v>
-      </c>
-      <c r="F42" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="43" spans="4:4">
-      <c r="B43" t="s">
-        <v>190</v>
-      </c>
-      <c r="C43" t="s">
-        <v>88</v>
-      </c>
-      <c r="D43" t="s">
-        <v>62</v>
-      </c>
-      <c r="E43" t="s">
-        <v>180</v>
-      </c>
-      <c r="F43" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="44" spans="4:4">
-      <c r="B44" t="s">
-        <v>191</v>
-      </c>
-      <c r="C44" t="s">
-        <v>88</v>
-      </c>
-      <c r="D44" t="s">
-        <v>62</v>
-      </c>
-      <c r="E44" t="s">
-        <v>74</v>
-      </c>
-      <c r="F44" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="45" spans="4:4">
-      <c r="B45" t="s">
-        <v>192</v>
-      </c>
-      <c r="C45" t="s">
-        <v>88</v>
-      </c>
-      <c r="D45" t="s">
-        <v>62</v>
-      </c>
-      <c r="E45" t="s">
-        <v>180</v>
-      </c>
-      <c r="F45" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="46" spans="4:4">
-      <c r="B46" t="s">
-        <v>193</v>
-      </c>
-      <c r="C46" t="s">
-        <v>88</v>
-      </c>
-      <c r="D46" t="s">
-        <v>62</v>
-      </c>
-      <c r="E46" t="s">
-        <v>74</v>
-      </c>
-      <c r="F46" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="47" spans="4:4">
-      <c r="B47" t="s">
-        <v>194</v>
-      </c>
-      <c r="C47" t="s">
-        <v>88</v>
-      </c>
-      <c r="D47" t="s">
-        <v>62</v>
-      </c>
-      <c r="E47" t="s">
-        <v>180</v>
-      </c>
-      <c r="F47" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="48" spans="4:4">
-      <c r="B48" t="s">
-        <v>195</v>
-      </c>
-      <c r="C48" t="s">
-        <v>88</v>
-      </c>
-      <c r="D48" t="s">
-        <v>62</v>
-      </c>
-      <c r="E48" t="s">
-        <v>196</v>
-      </c>
-      <c r="F48" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="49" spans="4:4">
-      <c r="B49" t="s">
-        <v>197</v>
-      </c>
-      <c r="C49" t="s">
-        <v>88</v>
-      </c>
-      <c r="D49" t="s">
-        <v>62</v>
-      </c>
-      <c r="E49" t="s">
-        <v>198</v>
-      </c>
-      <c r="F49" t="s">
-        <v>59</v>
-      </c>
-    </row>
+    <row r="40" spans="4:4"/>
+    <row r="41" spans="4:4"/>
+    <row r="42" spans="4:4"/>
+    <row r="43" spans="4:4"/>
+    <row r="44" spans="4:4"/>
+    <row r="45" spans="4:4"/>
+    <row r="46" spans="4:4"/>
+    <row r="47" spans="4:4"/>
+    <row r="48" spans="4:4"/>
+    <row r="49" spans="4:4"/>
     <row r="50" spans="4:4"/>
     <row r="51" spans="4:4"/>
     <row r="52" spans="4:4"/>

</xml_diff>

<commit_message>
Change russian text to svg_2
</commit_message>
<xml_diff>
--- a/t_12/TouchGFX/assets/texts/texts.xlsx
+++ b/t_12/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9935" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10101" uniqueCount="199">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2496,7 +2496,7 @@
     </row>
     <row r="26" spans="4:4">
       <c r="B26" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="C26" t="s">
         <v>88</v>
@@ -2505,7 +2505,7 @@
         <v>62</v>
       </c>
       <c r="E26" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="F26" t="s">
         <v>59</v>
@@ -2513,7 +2513,7 @@
     </row>
     <row r="27" spans="4:4">
       <c r="B27" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="C27" t="s">
         <v>88</v>
@@ -2522,216 +2522,24 @@
         <v>62</v>
       </c>
       <c r="E27" t="s">
-        <v>63</v>
+        <v>180</v>
       </c>
       <c r="F27" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="4:4">
-      <c r="B28" t="s">
-        <v>183</v>
-      </c>
-      <c r="C28" t="s">
-        <v>88</v>
-      </c>
-      <c r="D28" t="s">
-        <v>62</v>
-      </c>
-      <c r="E28" t="s">
-        <v>94</v>
-      </c>
-      <c r="F28" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="4:4">
-      <c r="B29" t="s">
-        <v>184</v>
-      </c>
-      <c r="C29" t="s">
-        <v>88</v>
-      </c>
-      <c r="D29" t="s">
-        <v>62</v>
-      </c>
-      <c r="E29" t="s">
-        <v>63</v>
-      </c>
-      <c r="F29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="4:4">
-      <c r="B30" t="s">
-        <v>185</v>
-      </c>
-      <c r="C30" t="s">
-        <v>88</v>
-      </c>
-      <c r="D30" t="s">
-        <v>62</v>
-      </c>
-      <c r="E30" t="s">
-        <v>94</v>
-      </c>
-      <c r="F30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="4:4">
-      <c r="B31" t="s">
-        <v>186</v>
-      </c>
-      <c r="C31" t="s">
-        <v>88</v>
-      </c>
-      <c r="D31" t="s">
-        <v>62</v>
-      </c>
-      <c r="E31" t="s">
-        <v>63</v>
-      </c>
-      <c r="F31" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="4:4">
-      <c r="B32" t="s">
-        <v>187</v>
-      </c>
-      <c r="C32" t="s">
-        <v>88</v>
-      </c>
-      <c r="D32" t="s">
-        <v>62</v>
-      </c>
-      <c r="E32" t="s">
-        <v>74</v>
-      </c>
-      <c r="F32" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="4:4">
-      <c r="B33" t="s">
-        <v>188</v>
-      </c>
-      <c r="C33" t="s">
-        <v>88</v>
-      </c>
-      <c r="D33" t="s">
-        <v>62</v>
-      </c>
-      <c r="E33" t="s">
-        <v>180</v>
-      </c>
-      <c r="F33" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="4:4">
-      <c r="B34" t="s">
-        <v>189</v>
-      </c>
-      <c r="C34" t="s">
-        <v>88</v>
-      </c>
-      <c r="D34" t="s">
-        <v>62</v>
-      </c>
-      <c r="E34" t="s">
-        <v>74</v>
-      </c>
-      <c r="F34" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="35" spans="4:4">
-      <c r="B35" t="s">
-        <v>190</v>
-      </c>
-      <c r="C35" t="s">
-        <v>88</v>
-      </c>
-      <c r="D35" t="s">
-        <v>62</v>
-      </c>
-      <c r="E35" t="s">
-        <v>180</v>
-      </c>
-      <c r="F35" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="4:4">
-      <c r="B36" t="s">
-        <v>191</v>
-      </c>
-      <c r="C36" t="s">
-        <v>88</v>
-      </c>
-      <c r="D36" t="s">
-        <v>62</v>
-      </c>
-      <c r="E36" t="s">
-        <v>74</v>
-      </c>
-      <c r="F36" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="4:4">
-      <c r="B37" t="s">
-        <v>192</v>
-      </c>
-      <c r="C37" t="s">
-        <v>88</v>
-      </c>
-      <c r="D37" t="s">
-        <v>62</v>
-      </c>
-      <c r="E37" t="s">
-        <v>180</v>
-      </c>
-      <c r="F37" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="38" spans="4:4">
-      <c r="B38" t="s">
-        <v>193</v>
-      </c>
-      <c r="C38" t="s">
-        <v>88</v>
-      </c>
-      <c r="D38" t="s">
-        <v>62</v>
-      </c>
-      <c r="E38" t="s">
-        <v>74</v>
-      </c>
-      <c r="F38" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="39" spans="4:4">
-      <c r="B39" t="s">
-        <v>194</v>
-      </c>
-      <c r="C39" t="s">
-        <v>88</v>
-      </c>
-      <c r="D39" t="s">
-        <v>62</v>
-      </c>
-      <c r="E39" t="s">
-        <v>180</v>
-      </c>
-      <c r="F39" t="s">
-        <v>59</v>
-      </c>
-    </row>
+    <row r="28" spans="4:4"/>
+    <row r="29" spans="4:4"/>
+    <row r="30" spans="4:4"/>
+    <row r="31" spans="4:4"/>
+    <row r="32" spans="4:4"/>
+    <row r="33" spans="4:4"/>
+    <row r="34" spans="4:4"/>
+    <row r="35" spans="4:4"/>
+    <row r="36" spans="4:4"/>
+    <row r="37" spans="4:4"/>
+    <row r="38" spans="4:4"/>
+    <row r="39" spans="4:4"/>
     <row r="40" spans="4:4"/>
     <row r="41" spans="4:4"/>
     <row r="42" spans="4:4"/>

</xml_diff>

<commit_message>
Change russian text to svg_5
</commit_message>
<xml_diff>
--- a/t_12/TouchGFX/assets/texts/texts.xlsx
+++ b/t_12/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10101" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10436" uniqueCount="201">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -614,6 +614,12 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;text&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SourceSansPro-Regular.ttf</t>
   </si>
 </sst>
 </file>
@@ -1991,6 +1997,25 @@
       </c>
     </row>
     <row r="8" spans="2:15">
+      <c r="B8" t="s">
+        <v>199</v>
+      </c>
+      <c r="C8" t="s">
+        <v>200</v>
+      </c>
+      <c r="D8">
+        <v>18</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
       <c r="K8" s="8" t="s">
         <v>16</v>
       </c>
@@ -2139,16 +2164,16 @@
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1">
       <c r="B5" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>94</v>
+        <v>52</v>
       </c>
       <c r="F5" t="s">
         <v>59</v>
@@ -2156,10 +2181,10 @@
     </row>
     <row r="6" spans="2:10">
       <c r="B6" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="D6" t="s">
         <v>58</v>
@@ -2173,16 +2198,16 @@
     </row>
     <row r="7" spans="2:10">
       <c r="B7" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="C7" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="D7" t="s">
         <v>58</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="F7" t="s">
         <v>59</v>
@@ -2190,7 +2215,7 @@
     </row>
     <row r="8" spans="2:10">
       <c r="B8" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="C8" t="s">
         <v>88</v>
@@ -2199,7 +2224,7 @@
         <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F8" t="s">
         <v>59</v>
@@ -2207,16 +2232,16 @@
     </row>
     <row r="9" spans="2:10">
       <c r="B9" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="F9" t="s">
         <v>59</v>
@@ -2224,7 +2249,7 @@
     </row>
     <row r="10" spans="2:10">
       <c r="B10" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C10" t="s">
         <v>88</v>
@@ -2233,7 +2258,7 @@
         <v>62</v>
       </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="F10" t="s">
         <v>59</v>
@@ -2241,7 +2266,7 @@
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C11" t="s">
         <v>88</v>
@@ -2250,7 +2275,7 @@
         <v>62</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>121</v>
       </c>
       <c r="F11" t="s">
         <v>59</v>
@@ -2258,7 +2283,7 @@
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="C12" t="s">
         <v>88</v>
@@ -2267,7 +2292,7 @@
         <v>62</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>121</v>
       </c>
       <c r="F12" t="s">
         <v>59</v>
@@ -2275,16 +2300,16 @@
     </row>
     <row r="13" spans="2:10">
       <c r="B13" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="C13" t="s">
-        <v>88</v>
+        <v>199</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E13" t="s">
-        <v>121</v>
+        <v>46</v>
       </c>
       <c r="F13" t="s">
         <v>59</v>
@@ -2292,16 +2317,16 @@
     </row>
     <row r="14" spans="2:10">
       <c r="B14" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C14" t="s">
-        <v>88</v>
+        <v>199</v>
       </c>
       <c r="D14" t="s">
         <v>62</v>
       </c>
       <c r="E14" t="s">
-        <v>121</v>
+        <v>166</v>
       </c>
       <c r="F14" t="s">
         <v>59</v>
@@ -2309,10 +2334,10 @@
     </row>
     <row r="15" spans="2:10">
       <c r="B15" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="C15" t="s">
-        <v>88</v>
+        <v>199</v>
       </c>
       <c r="D15" t="s">
         <v>58</v>
@@ -2326,10 +2351,10 @@
     </row>
     <row r="16" spans="2:10">
       <c r="B16" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
       <c r="C16" t="s">
-        <v>88</v>
+        <v>199</v>
       </c>
       <c r="D16" t="s">
         <v>62</v>
@@ -2343,10 +2368,10 @@
     </row>
     <row r="17" spans="4:4">
       <c r="B17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C17" t="s">
-        <v>88</v>
+        <v>199</v>
       </c>
       <c r="D17" t="s">
         <v>58</v>
@@ -2360,10 +2385,10 @@
     </row>
     <row r="18" spans="4:4">
       <c r="B18" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C18" t="s">
-        <v>88</v>
+        <v>199</v>
       </c>
       <c r="D18" t="s">
         <v>62</v>
@@ -2377,10 +2402,10 @@
     </row>
     <row r="19" spans="4:4">
       <c r="B19" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C19" t="s">
-        <v>88</v>
+        <v>199</v>
       </c>
       <c r="D19" t="s">
         <v>58</v>
@@ -2394,10 +2419,10 @@
     </row>
     <row r="20" spans="4:4">
       <c r="B20" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C20" t="s">
-        <v>88</v>
+        <v>199</v>
       </c>
       <c r="D20" t="s">
         <v>62</v>
@@ -2411,16 +2436,16 @@
     </row>
     <row r="21" spans="4:4">
       <c r="B21" t="s">
-        <v>152</v>
+        <v>176</v>
       </c>
       <c r="C21" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="D21" t="s">
         <v>58</v>
       </c>
       <c r="E21" t="s">
-        <v>46</v>
+        <v>177</v>
       </c>
       <c r="F21" t="s">
         <v>59</v>
@@ -2428,16 +2453,16 @@
     </row>
     <row r="22" spans="4:4">
       <c r="B22" t="s">
-        <v>153</v>
+        <v>178</v>
       </c>
       <c r="C22" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E22" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="F22" t="s">
         <v>59</v>
@@ -2445,16 +2470,16 @@
     </row>
     <row r="23" spans="4:4">
       <c r="B23" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="D23" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E23" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="F23" t="s">
         <v>59</v>
@@ -2462,16 +2487,16 @@
     </row>
     <row r="24" spans="4:4">
       <c r="B24" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="D24" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E24" t="s">
-        <v>177</v>
+        <v>74</v>
       </c>
       <c r="F24" t="s">
         <v>59</v>
@@ -2479,7 +2504,7 @@
     </row>
     <row r="25" spans="4:4">
       <c r="B25" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="C25" t="s">
         <v>88</v>
@@ -2496,7 +2521,7 @@
     </row>
     <row r="26" spans="4:4">
       <c r="B26" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C26" t="s">
         <v>88</v>
@@ -2505,7 +2530,7 @@
         <v>62</v>
       </c>
       <c r="E26" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="F26" t="s">
         <v>59</v>
@@ -2513,7 +2538,7 @@
     </row>
     <row r="27" spans="4:4">
       <c r="B27" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C27" t="s">
         <v>88</v>
@@ -2522,7 +2547,7 @@
         <v>62</v>
       </c>
       <c r="E27" t="s">
-        <v>180</v>
+        <v>63</v>
       </c>
       <c r="F27" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
Change img to fonts_0
</commit_message>
<xml_diff>
--- a/t_12/TouchGFX/assets/texts/texts.xlsx
+++ b/t_12/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10436" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15018" uniqueCount="259">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -620,6 +620,180 @@
   </si>
   <si>
     <t xml:space="preserve">SourceSansPro-Regular.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELHART</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logo_M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId92</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DI_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b_DI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DI_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DI_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DI_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DO_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DO_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DO_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DO_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b_Screens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arial.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId108</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set Points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graphic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analytics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Archive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discret</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analog inputs #1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dd/mm/yyyy</t>
   </si>
 </sst>
 </file>
@@ -1854,7 +2028,7 @@
         <v>53</v>
       </c>
       <c r="D4">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -1927,7 +2101,7 @@
         <v>88</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="D6">
         <v>20</v>
@@ -1962,13 +2136,13 @@
     </row>
     <row r="7" spans="2:15">
       <c r="B7" t="s">
-        <v>108</v>
+        <v>201</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="D7">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E7">
         <v>4</v>
@@ -2031,6 +2205,25 @@
       <c r="O8" s="11"/>
     </row>
     <row r="9" spans="2:15">
+      <c r="B9" t="s">
+        <v>204</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9">
+        <v>30</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
       <c r="K9" s="12" t="s">
         <v>14</v>
       </c>
@@ -2048,6 +2241,25 @@
       </c>
     </row>
     <row r="10" spans="2:15">
+      <c r="B10" t="s">
+        <v>205</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10">
+        <v>25</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
       <c r="K10" s="12" t="s">
         <v>36</v>
       </c>
@@ -2063,9 +2275,47 @@
       <c r="O10" s="15"/>
     </row>
     <row r="11" spans="2:15">
+      <c r="B11" t="s">
+        <v>215</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
       <c r="K11" s="16"/>
     </row>
     <row r="12" spans="2:15">
+      <c r="B12" t="s">
+        <v>238</v>
+      </c>
+      <c r="C12" t="s">
+        <v>239</v>
+      </c>
+      <c r="D12">
+        <v>12</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
       <c r="L12" s="17" t="s">
         <v>35</v>
       </c>
@@ -2201,7 +2451,7 @@
         <v>109</v>
       </c>
       <c r="C7" t="s">
-        <v>108</v>
+        <v>201</v>
       </c>
       <c r="D7" t="s">
         <v>58</v>
@@ -2470,7 +2720,7 @@
     </row>
     <row r="23" spans="4:4">
       <c r="B23" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="C23" t="s">
         <v>88</v>
@@ -2479,7 +2729,7 @@
         <v>62</v>
       </c>
       <c r="E23" t="s">
-        <v>180</v>
+        <v>74</v>
       </c>
       <c r="F23" t="s">
         <v>59</v>
@@ -2487,7 +2737,7 @@
     </row>
     <row r="24" spans="4:4">
       <c r="B24" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C24" t="s">
         <v>88</v>
@@ -2496,7 +2746,7 @@
         <v>62</v>
       </c>
       <c r="E24" t="s">
-        <v>74</v>
+        <v>180</v>
       </c>
       <c r="F24" t="s">
         <v>59</v>
@@ -2504,7 +2754,7 @@
     </row>
     <row r="25" spans="4:4">
       <c r="B25" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C25" t="s">
         <v>88</v>
@@ -2513,7 +2763,7 @@
         <v>62</v>
       </c>
       <c r="E25" t="s">
-        <v>180</v>
+        <v>94</v>
       </c>
       <c r="F25" t="s">
         <v>59</v>
@@ -2521,7 +2771,7 @@
     </row>
     <row r="26" spans="4:4">
       <c r="B26" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C26" t="s">
         <v>88</v>
@@ -2530,7 +2780,7 @@
         <v>62</v>
       </c>
       <c r="E26" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="F26" t="s">
         <v>59</v>
@@ -2538,57 +2788,633 @@
     </row>
     <row r="27" spans="4:4">
       <c r="B27" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C27" t="s">
-        <v>88</v>
+        <v>201</v>
       </c>
       <c r="D27" t="s">
         <v>62</v>
       </c>
       <c r="E27" t="s">
-        <v>63</v>
+        <v>201</v>
       </c>
       <c r="F27" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="4:4"/>
-    <row r="29" spans="4:4"/>
-    <row r="30" spans="4:4"/>
-    <row r="31" spans="4:4"/>
-    <row r="32" spans="4:4"/>
-    <row r="33" spans="4:4"/>
-    <row r="34" spans="4:4"/>
-    <row r="35" spans="4:4"/>
-    <row r="36" spans="4:4"/>
-    <row r="37" spans="4:4"/>
-    <row r="38" spans="4:4"/>
-    <row r="39" spans="4:4"/>
-    <row r="40" spans="4:4"/>
-    <row r="41" spans="4:4"/>
-    <row r="42" spans="4:4"/>
-    <row r="43" spans="4:4"/>
-    <row r="44" spans="4:4"/>
-    <row r="45" spans="4:4"/>
-    <row r="46" spans="4:4"/>
-    <row r="47" spans="4:4"/>
-    <row r="48" spans="4:4"/>
-    <row r="49" spans="4:4"/>
-    <row r="50" spans="4:4"/>
-    <row r="51" spans="4:4"/>
-    <row r="52" spans="4:4"/>
-    <row r="53" spans="4:4"/>
-    <row r="54" spans="4:4"/>
-    <row r="55" spans="4:4"/>
-    <row r="56" spans="4:4"/>
-    <row r="57" spans="4:4"/>
-    <row r="58" spans="4:4"/>
-    <row r="59" spans="4:4"/>
-    <row r="60" spans="4:4"/>
-    <row r="61" spans="4:4"/>
-    <row r="62" spans="4:4"/>
-    <row r="63" spans="4:4"/>
+    <row r="28" spans="4:4">
+      <c r="B28" t="s">
+        <v>192</v>
+      </c>
+      <c r="C28" t="s">
+        <v>201</v>
+      </c>
+      <c r="D28" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" t="s">
+        <v>202</v>
+      </c>
+      <c r="F28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4">
+      <c r="B29" t="s">
+        <v>193</v>
+      </c>
+      <c r="C29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" t="s">
+        <v>203</v>
+      </c>
+      <c r="F29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="4:4">
+      <c r="B30" t="s">
+        <v>194</v>
+      </c>
+      <c r="C30" t="s">
+        <v>204</v>
+      </c>
+      <c r="D30" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" t="s">
+        <v>203</v>
+      </c>
+      <c r="F30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4">
+      <c r="B31" t="s">
+        <v>195</v>
+      </c>
+      <c r="C31" t="s">
+        <v>204</v>
+      </c>
+      <c r="D31" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" t="s">
+        <v>203</v>
+      </c>
+      <c r="F31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="4:4">
+      <c r="B32" t="s">
+        <v>197</v>
+      </c>
+      <c r="C32" t="s">
+        <v>205</v>
+      </c>
+      <c r="D32" t="s">
+        <v>62</v>
+      </c>
+      <c r="E32" t="s">
+        <v>206</v>
+      </c>
+      <c r="F32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4">
+      <c r="B33" t="s">
+        <v>207</v>
+      </c>
+      <c r="C33" t="s">
+        <v>205</v>
+      </c>
+      <c r="D33" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33" t="s">
+        <v>208</v>
+      </c>
+      <c r="F33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4">
+      <c r="B34" t="s">
+        <v>209</v>
+      </c>
+      <c r="C34" t="s">
+        <v>205</v>
+      </c>
+      <c r="D34" t="s">
+        <v>62</v>
+      </c>
+      <c r="E34" t="s">
+        <v>210</v>
+      </c>
+      <c r="F34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4">
+      <c r="B35" t="s">
+        <v>211</v>
+      </c>
+      <c r="C35" t="s">
+        <v>205</v>
+      </c>
+      <c r="D35" t="s">
+        <v>62</v>
+      </c>
+      <c r="E35" t="s">
+        <v>212</v>
+      </c>
+      <c r="F35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4">
+      <c r="B36" t="s">
+        <v>213</v>
+      </c>
+      <c r="C36" t="s">
+        <v>215</v>
+      </c>
+      <c r="D36" t="s">
+        <v>58</v>
+      </c>
+      <c r="E36" t="s">
+        <v>214</v>
+      </c>
+      <c r="F36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4">
+      <c r="B37" t="s">
+        <v>216</v>
+      </c>
+      <c r="C37" t="s">
+        <v>215</v>
+      </c>
+      <c r="D37" t="s">
+        <v>58</v>
+      </c>
+      <c r="E37" t="s">
+        <v>217</v>
+      </c>
+      <c r="F37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4">
+      <c r="B38" t="s">
+        <v>218</v>
+      </c>
+      <c r="C38" t="s">
+        <v>215</v>
+      </c>
+      <c r="D38" t="s">
+        <v>58</v>
+      </c>
+      <c r="E38" t="s">
+        <v>219</v>
+      </c>
+      <c r="F38" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4">
+      <c r="B39" t="s">
+        <v>220</v>
+      </c>
+      <c r="C39" t="s">
+        <v>215</v>
+      </c>
+      <c r="D39" t="s">
+        <v>58</v>
+      </c>
+      <c r="E39" t="s">
+        <v>221</v>
+      </c>
+      <c r="F39" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4">
+      <c r="B40" t="s">
+        <v>222</v>
+      </c>
+      <c r="C40" t="s">
+        <v>215</v>
+      </c>
+      <c r="D40" t="s">
+        <v>58</v>
+      </c>
+      <c r="E40" t="s">
+        <v>223</v>
+      </c>
+      <c r="F40" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4">
+      <c r="B41" t="s">
+        <v>224</v>
+      </c>
+      <c r="C41" t="s">
+        <v>215</v>
+      </c>
+      <c r="D41" t="s">
+        <v>58</v>
+      </c>
+      <c r="E41" t="s">
+        <v>225</v>
+      </c>
+      <c r="F41" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4">
+      <c r="B42" t="s">
+        <v>226</v>
+      </c>
+      <c r="C42" t="s">
+        <v>215</v>
+      </c>
+      <c r="D42" t="s">
+        <v>58</v>
+      </c>
+      <c r="E42" t="s">
+        <v>227</v>
+      </c>
+      <c r="F42" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4">
+      <c r="B43" t="s">
+        <v>228</v>
+      </c>
+      <c r="C43" t="s">
+        <v>215</v>
+      </c>
+      <c r="D43" t="s">
+        <v>58</v>
+      </c>
+      <c r="E43" t="s">
+        <v>229</v>
+      </c>
+      <c r="F43" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="4:4">
+      <c r="B44" t="s">
+        <v>230</v>
+      </c>
+      <c r="C44" t="s">
+        <v>215</v>
+      </c>
+      <c r="D44" t="s">
+        <v>58</v>
+      </c>
+      <c r="E44" t="s">
+        <v>214</v>
+      </c>
+      <c r="F44" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4">
+      <c r="B45" t="s">
+        <v>231</v>
+      </c>
+      <c r="C45" t="s">
+        <v>215</v>
+      </c>
+      <c r="D45" t="s">
+        <v>58</v>
+      </c>
+      <c r="E45" t="s">
+        <v>217</v>
+      </c>
+      <c r="F45" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="4:4">
+      <c r="B46" t="s">
+        <v>232</v>
+      </c>
+      <c r="C46" t="s">
+        <v>215</v>
+      </c>
+      <c r="D46" t="s">
+        <v>58</v>
+      </c>
+      <c r="E46" t="s">
+        <v>219</v>
+      </c>
+      <c r="F46" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="4:4">
+      <c r="B47" t="s">
+        <v>233</v>
+      </c>
+      <c r="C47" t="s">
+        <v>215</v>
+      </c>
+      <c r="D47" t="s">
+        <v>58</v>
+      </c>
+      <c r="E47" t="s">
+        <v>221</v>
+      </c>
+      <c r="F47" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="4:4">
+      <c r="B48" t="s">
+        <v>234</v>
+      </c>
+      <c r="C48" t="s">
+        <v>215</v>
+      </c>
+      <c r="D48" t="s">
+        <v>58</v>
+      </c>
+      <c r="E48" t="s">
+        <v>223</v>
+      </c>
+      <c r="F48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4">
+      <c r="B49" t="s">
+        <v>235</v>
+      </c>
+      <c r="C49" t="s">
+        <v>215</v>
+      </c>
+      <c r="D49" t="s">
+        <v>58</v>
+      </c>
+      <c r="E49" t="s">
+        <v>225</v>
+      </c>
+      <c r="F49" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4">
+      <c r="B50" t="s">
+        <v>236</v>
+      </c>
+      <c r="C50" t="s">
+        <v>215</v>
+      </c>
+      <c r="D50" t="s">
+        <v>58</v>
+      </c>
+      <c r="E50" t="s">
+        <v>227</v>
+      </c>
+      <c r="F50" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4">
+      <c r="B51" t="s">
+        <v>237</v>
+      </c>
+      <c r="C51" t="s">
+        <v>215</v>
+      </c>
+      <c r="D51" t="s">
+        <v>58</v>
+      </c>
+      <c r="E51" t="s">
+        <v>229</v>
+      </c>
+      <c r="F51" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="52" spans="4:4">
+      <c r="B52" t="s">
+        <v>240</v>
+      </c>
+      <c r="C52" t="s">
+        <v>238</v>
+      </c>
+      <c r="D52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E52" t="s">
+        <v>201</v>
+      </c>
+      <c r="F52" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53" spans="4:4">
+      <c r="B53" t="s">
+        <v>241</v>
+      </c>
+      <c r="C53" t="s">
+        <v>238</v>
+      </c>
+      <c r="D53" t="s">
+        <v>58</v>
+      </c>
+      <c r="E53" t="s">
+        <v>242</v>
+      </c>
+      <c r="F53" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="4:4">
+      <c r="B54" t="s">
+        <v>243</v>
+      </c>
+      <c r="C54" t="s">
+        <v>238</v>
+      </c>
+      <c r="D54" t="s">
+        <v>58</v>
+      </c>
+      <c r="E54" t="s">
+        <v>244</v>
+      </c>
+      <c r="F54" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="4:4">
+      <c r="B55" t="s">
+        <v>245</v>
+      </c>
+      <c r="C55" t="s">
+        <v>238</v>
+      </c>
+      <c r="D55" t="s">
+        <v>58</v>
+      </c>
+      <c r="E55" t="s">
+        <v>246</v>
+      </c>
+      <c r="F55" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="4:4">
+      <c r="B56" t="s">
+        <v>247</v>
+      </c>
+      <c r="C56" t="s">
+        <v>238</v>
+      </c>
+      <c r="D56" t="s">
+        <v>58</v>
+      </c>
+      <c r="E56" t="s">
+        <v>248</v>
+      </c>
+      <c r="F56" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="4:4">
+      <c r="B57" t="s">
+        <v>249</v>
+      </c>
+      <c r="C57" t="s">
+        <v>238</v>
+      </c>
+      <c r="D57" t="s">
+        <v>58</v>
+      </c>
+      <c r="E57" t="s">
+        <v>201</v>
+      </c>
+      <c r="F57" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="4:4">
+      <c r="B58" t="s">
+        <v>250</v>
+      </c>
+      <c r="C58" t="s">
+        <v>238</v>
+      </c>
+      <c r="D58" t="s">
+        <v>58</v>
+      </c>
+      <c r="E58" t="s">
+        <v>242</v>
+      </c>
+      <c r="F58" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="4:4">
+      <c r="B59" t="s">
+        <v>251</v>
+      </c>
+      <c r="C59" t="s">
+        <v>238</v>
+      </c>
+      <c r="D59" t="s">
+        <v>58</v>
+      </c>
+      <c r="E59" t="s">
+        <v>252</v>
+      </c>
+      <c r="F59" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="4:4">
+      <c r="B60" t="s">
+        <v>253</v>
+      </c>
+      <c r="C60" t="s">
+        <v>238</v>
+      </c>
+      <c r="D60" t="s">
+        <v>58</v>
+      </c>
+      <c r="E60" t="s">
+        <v>246</v>
+      </c>
+      <c r="F60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="4:4">
+      <c r="B61" t="s">
+        <v>254</v>
+      </c>
+      <c r="C61" t="s">
+        <v>238</v>
+      </c>
+      <c r="D61" t="s">
+        <v>58</v>
+      </c>
+      <c r="E61" t="s">
+        <v>248</v>
+      </c>
+      <c r="F61" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="4:4">
+      <c r="B62" t="s">
+        <v>255</v>
+      </c>
+      <c r="C62" t="s">
+        <v>88</v>
+      </c>
+      <c r="D62" t="s">
+        <v>62</v>
+      </c>
+      <c r="E62" t="s">
+        <v>256</v>
+      </c>
+      <c r="F62" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="4:4">
+      <c r="B63" t="s">
+        <v>257</v>
+      </c>
+      <c r="C63" t="s">
+        <v>88</v>
+      </c>
+      <c r="D63" t="s">
+        <v>62</v>
+      </c>
+      <c r="E63" t="s">
+        <v>258</v>
+      </c>
+      <c r="F63" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="64" spans="4:4"/>
     <row r="65" spans="4:4"/>
     <row r="66" spans="4:4"/>

</xml_diff>

<commit_message>
W. Found right version of program
</commit_message>
<xml_diff>
--- a/t_12/TouchGFX/assets/texts/texts.xlsx
+++ b/t_12/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10436" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10101" uniqueCount="199">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -614,12 +614,6 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;text&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AI_value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SourceSansPro-Regular.ttf</t>
   </si>
 </sst>
 </file>
@@ -1997,25 +1991,6 @@
       </c>
     </row>
     <row r="8" spans="2:15">
-      <c r="B8" t="s">
-        <v>199</v>
-      </c>
-      <c r="C8" t="s">
-        <v>200</v>
-      </c>
-      <c r="D8">
-        <v>18</v>
-      </c>
-      <c r="E8">
-        <v>4</v>
-      </c>
-      <c r="F8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8"/>
-      <c r="J8"/>
       <c r="K8" s="8" t="s">
         <v>16</v>
       </c>
@@ -2164,16 +2139,16 @@
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1">
       <c r="B5" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>94</v>
       </c>
       <c r="F5" t="s">
         <v>59</v>
@@ -2181,10 +2156,10 @@
     </row>
     <row r="6" spans="2:10">
       <c r="B6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
         <v>58</v>
@@ -2198,16 +2173,16 @@
     </row>
     <row r="7" spans="2:10">
       <c r="B7" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="D7" t="s">
         <v>58</v>
       </c>
       <c r="E7" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="F7" t="s">
         <v>59</v>
@@ -2215,7 +2190,7 @@
     </row>
     <row r="8" spans="2:10">
       <c r="B8" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="C8" t="s">
         <v>88</v>
@@ -2224,7 +2199,7 @@
         <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="F8" t="s">
         <v>59</v>
@@ -2232,16 +2207,16 @@
     </row>
     <row r="9" spans="2:10">
       <c r="B9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C9" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="F9" t="s">
         <v>59</v>
@@ -2249,7 +2224,7 @@
     </row>
     <row r="10" spans="2:10">
       <c r="B10" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C10" t="s">
         <v>88</v>
@@ -2258,7 +2233,7 @@
         <v>62</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="F10" t="s">
         <v>59</v>
@@ -2266,7 +2241,7 @@
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C11" t="s">
         <v>88</v>
@@ -2275,7 +2250,7 @@
         <v>62</v>
       </c>
       <c r="E11" t="s">
-        <v>121</v>
+        <v>46</v>
       </c>
       <c r="F11" t="s">
         <v>59</v>
@@ -2283,7 +2258,7 @@
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C12" t="s">
         <v>88</v>
@@ -2292,7 +2267,7 @@
         <v>62</v>
       </c>
       <c r="E12" t="s">
-        <v>121</v>
+        <v>46</v>
       </c>
       <c r="F12" t="s">
         <v>59</v>
@@ -2300,16 +2275,16 @@
     </row>
     <row r="13" spans="2:10">
       <c r="B13" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C13" t="s">
-        <v>199</v>
+        <v>88</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>121</v>
       </c>
       <c r="F13" t="s">
         <v>59</v>
@@ -2317,16 +2292,16 @@
     </row>
     <row r="14" spans="2:10">
       <c r="B14" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C14" t="s">
-        <v>199</v>
+        <v>88</v>
       </c>
       <c r="D14" t="s">
         <v>62</v>
       </c>
       <c r="E14" t="s">
-        <v>166</v>
+        <v>121</v>
       </c>
       <c r="F14" t="s">
         <v>59</v>
@@ -2334,10 +2309,10 @@
     </row>
     <row r="15" spans="2:10">
       <c r="B15" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="C15" t="s">
-        <v>199</v>
+        <v>88</v>
       </c>
       <c r="D15" t="s">
         <v>58</v>
@@ -2351,10 +2326,10 @@
     </row>
     <row r="16" spans="2:10">
       <c r="B16" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
       <c r="C16" t="s">
-        <v>199</v>
+        <v>88</v>
       </c>
       <c r="D16" t="s">
         <v>62</v>
@@ -2368,10 +2343,10 @@
     </row>
     <row r="17" spans="4:4">
       <c r="B17" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C17" t="s">
-        <v>199</v>
+        <v>88</v>
       </c>
       <c r="D17" t="s">
         <v>58</v>
@@ -2385,10 +2360,10 @@
     </row>
     <row r="18" spans="4:4">
       <c r="B18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C18" t="s">
-        <v>199</v>
+        <v>88</v>
       </c>
       <c r="D18" t="s">
         <v>62</v>
@@ -2402,10 +2377,10 @@
     </row>
     <row r="19" spans="4:4">
       <c r="B19" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C19" t="s">
-        <v>199</v>
+        <v>88</v>
       </c>
       <c r="D19" t="s">
         <v>58</v>
@@ -2419,10 +2394,10 @@
     </row>
     <row r="20" spans="4:4">
       <c r="B20" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C20" t="s">
-        <v>199</v>
+        <v>88</v>
       </c>
       <c r="D20" t="s">
         <v>62</v>
@@ -2436,16 +2411,16 @@
     </row>
     <row r="21" spans="4:4">
       <c r="B21" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="D21" t="s">
         <v>58</v>
       </c>
       <c r="E21" t="s">
-        <v>177</v>
+        <v>46</v>
       </c>
       <c r="F21" t="s">
         <v>59</v>
@@ -2453,16 +2428,16 @@
     </row>
     <row r="22" spans="4:4">
       <c r="B22" t="s">
-        <v>178</v>
+        <v>153</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="D22" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E22" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="F22" t="s">
         <v>59</v>
@@ -2470,16 +2445,16 @@
     </row>
     <row r="23" spans="4:4">
       <c r="B23" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C23" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E23" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F23" t="s">
         <v>59</v>
@@ -2487,16 +2462,16 @@
     </row>
     <row r="24" spans="4:4">
       <c r="B24" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C24" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="D24" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E24" t="s">
-        <v>74</v>
+        <v>177</v>
       </c>
       <c r="F24" t="s">
         <v>59</v>
@@ -2504,7 +2479,7 @@
     </row>
     <row r="25" spans="4:4">
       <c r="B25" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="C25" t="s">
         <v>88</v>
@@ -2521,7 +2496,7 @@
     </row>
     <row r="26" spans="4:4">
       <c r="B26" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C26" t="s">
         <v>88</v>
@@ -2530,7 +2505,7 @@
         <v>62</v>
       </c>
       <c r="E26" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="F26" t="s">
         <v>59</v>
@@ -2538,7 +2513,7 @@
     </row>
     <row r="27" spans="4:4">
       <c r="B27" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C27" t="s">
         <v>88</v>
@@ -2547,7 +2522,7 @@
         <v>62</v>
       </c>
       <c r="E27" t="s">
-        <v>63</v>
+        <v>180</v>
       </c>
       <c r="F27" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
++++ AI is done!
</commit_message>
<xml_diff>
--- a/t_12/TouchGFX/assets/texts/texts.xlsx
+++ b/t_12/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10101" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10611" uniqueCount="199">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2479,7 +2479,7 @@
     </row>
     <row r="25" spans="4:4">
       <c r="B25" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="C25" t="s">
         <v>88</v>
@@ -2488,7 +2488,7 @@
         <v>62</v>
       </c>
       <c r="E25" t="s">
-        <v>180</v>
+        <v>74</v>
       </c>
       <c r="F25" t="s">
         <v>59</v>
@@ -2496,7 +2496,7 @@
     </row>
     <row r="26" spans="4:4">
       <c r="B26" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C26" t="s">
         <v>88</v>
@@ -2505,7 +2505,7 @@
         <v>62</v>
       </c>
       <c r="E26" t="s">
-        <v>74</v>
+        <v>180</v>
       </c>
       <c r="F26" t="s">
         <v>59</v>
@@ -2513,7 +2513,7 @@
     </row>
     <row r="27" spans="4:4">
       <c r="B27" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C27" t="s">
         <v>88</v>
@@ -2522,13 +2522,29 @@
         <v>62</v>
       </c>
       <c r="E27" t="s">
-        <v>180</v>
+        <v>46</v>
       </c>
       <c r="F27" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="4:4"/>
+    <row r="28" spans="4:4">
+      <c r="B28" t="s">
+        <v>190</v>
+      </c>
+      <c r="C28" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" t="s">
+        <v>180</v>
+      </c>
+      <c r="F28" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="29" spans="4:4"/>
     <row r="30" spans="4:4"/>
     <row r="31" spans="4:4"/>

</xml_diff>

<commit_message>
++++ Date is almost done!
</commit_message>
<xml_diff>
--- a/t_12/TouchGFX/assets/texts/texts.xlsx
+++ b/t_12/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10611" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11309" uniqueCount="201">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -614,6 +614,12 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;text&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t_AI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt; </t>
   </si>
 </sst>
 </file>
@@ -1991,6 +1997,27 @@
       </c>
     </row>
     <row r="8" spans="2:15">
+      <c r="B8" t="s">
+        <v>199</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8"/>
+      <c r="J8"/>
       <c r="K8" s="8" t="s">
         <v>16</v>
       </c>
@@ -2312,7 +2339,7 @@
         <v>124</v>
       </c>
       <c r="C15" t="s">
-        <v>88</v>
+        <v>199</v>
       </c>
       <c r="D15" t="s">
         <v>58</v>
@@ -2329,7 +2356,7 @@
         <v>125</v>
       </c>
       <c r="C16" t="s">
-        <v>88</v>
+        <v>199</v>
       </c>
       <c r="D16" t="s">
         <v>62</v>
@@ -2346,7 +2373,7 @@
         <v>148</v>
       </c>
       <c r="C17" t="s">
-        <v>88</v>
+        <v>199</v>
       </c>
       <c r="D17" t="s">
         <v>58</v>
@@ -2363,7 +2390,7 @@
         <v>149</v>
       </c>
       <c r="C18" t="s">
-        <v>88</v>
+        <v>199</v>
       </c>
       <c r="D18" t="s">
         <v>62</v>
@@ -2380,7 +2407,7 @@
         <v>150</v>
       </c>
       <c r="C19" t="s">
-        <v>88</v>
+        <v>199</v>
       </c>
       <c r="D19" t="s">
         <v>58</v>
@@ -2397,7 +2424,7 @@
         <v>151</v>
       </c>
       <c r="C20" t="s">
-        <v>88</v>
+        <v>199</v>
       </c>
       <c r="D20" t="s">
         <v>62</v>
@@ -2414,7 +2441,7 @@
         <v>152</v>
       </c>
       <c r="C21" t="s">
-        <v>88</v>
+        <v>199</v>
       </c>
       <c r="D21" t="s">
         <v>58</v>
@@ -2431,7 +2458,7 @@
         <v>153</v>
       </c>
       <c r="C22" t="s">
-        <v>88</v>
+        <v>199</v>
       </c>
       <c r="D22" t="s">
         <v>62</v>
@@ -2513,7 +2540,7 @@
     </row>
     <row r="27" spans="4:4">
       <c r="B27" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C27" t="s">
         <v>88</v>
@@ -2522,7 +2549,7 @@
         <v>62</v>
       </c>
       <c r="E27" t="s">
-        <v>46</v>
+        <v>200</v>
       </c>
       <c r="F27" t="s">
         <v>59</v>
@@ -2530,7 +2557,7 @@
     </row>
     <row r="28" spans="4:4">
       <c r="B28" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C28" t="s">
         <v>88</v>
@@ -2539,7 +2566,7 @@
         <v>62</v>
       </c>
       <c r="E28" t="s">
-        <v>180</v>
+        <v>63</v>
       </c>
       <c r="F28" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
Deleted second(dg_SP_AI_1) graphic from GUI
</commit_message>
<xml_diff>
--- a/t_12/TouchGFX/assets/texts/texts.xlsx
+++ b/t_12/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14707" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14959" uniqueCount="222">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2253,13 +2253,13 @@
         <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>199</v>
       </c>
       <c r="D5" t="s">
         <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>94</v>
+        <v>46</v>
       </c>
       <c r="F5" t="s">
         <v>59</v>
@@ -2304,7 +2304,7 @@
         <v>97</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
+        <v>199</v>
       </c>
       <c r="D8" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
Update GUI. Added radio buttons
</commit_message>
<xml_diff>
--- a/t_12/TouchGFX/assets/texts/texts.xlsx
+++ b/t_12/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14959" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16132" uniqueCount="236">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -683,6 +683,48 @@
   </si>
   <si>
     <t xml:space="preserve">Date_Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RB_Indicators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId119</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRG</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> :  &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> : &lt;value&gt;</t>
   </si>
 </sst>
 </file>
@@ -2134,6 +2176,25 @@
       </c>
     </row>
     <row r="10" spans="2:15">
+      <c r="B10" t="s">
+        <v>224</v>
+      </c>
+      <c r="C10" t="s">
+        <v>206</v>
+      </c>
+      <c r="D10">
+        <v>11</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
       <c r="K10" s="12" t="s">
         <v>36</v>
       </c>
@@ -2259,7 +2320,7 @@
         <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>235</v>
       </c>
       <c r="F5" t="s">
         <v>59</v>
@@ -2860,14 +2921,142 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="4:4"/>
-    <row r="42" spans="4:4"/>
-    <row r="43" spans="4:4"/>
-    <row r="44" spans="4:4"/>
-    <row r="45" spans="4:4"/>
-    <row r="46" spans="4:4"/>
-    <row r="47" spans="4:4"/>
-    <row r="48" spans="4:4"/>
+    <row r="41" spans="4:4">
+      <c r="B41" t="s">
+        <v>222</v>
+      </c>
+      <c r="C41" t="s">
+        <v>199</v>
+      </c>
+      <c r="D41" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F41" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4">
+      <c r="B42" t="s">
+        <v>223</v>
+      </c>
+      <c r="C42" t="s">
+        <v>199</v>
+      </c>
+      <c r="D42" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42" t="s">
+        <v>63</v>
+      </c>
+      <c r="F42" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4">
+      <c r="B43" t="s">
+        <v>225</v>
+      </c>
+      <c r="C43" t="s">
+        <v>224</v>
+      </c>
+      <c r="D43" t="s">
+        <v>58</v>
+      </c>
+      <c r="E43" t="s">
+        <v>200</v>
+      </c>
+      <c r="F43" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="4:4">
+      <c r="B44" t="s">
+        <v>226</v>
+      </c>
+      <c r="C44" t="s">
+        <v>224</v>
+      </c>
+      <c r="D44" t="s">
+        <v>62</v>
+      </c>
+      <c r="E44" t="s">
+        <v>227</v>
+      </c>
+      <c r="F44" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4">
+      <c r="B45" t="s">
+        <v>228</v>
+      </c>
+      <c r="C45" t="s">
+        <v>224</v>
+      </c>
+      <c r="D45" t="s">
+        <v>58</v>
+      </c>
+      <c r="E45" t="s">
+        <v>200</v>
+      </c>
+      <c r="F45" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="4:4">
+      <c r="B46" t="s">
+        <v>229</v>
+      </c>
+      <c r="C46" t="s">
+        <v>224</v>
+      </c>
+      <c r="D46" t="s">
+        <v>62</v>
+      </c>
+      <c r="E46" t="s">
+        <v>230</v>
+      </c>
+      <c r="F46" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="4:4">
+      <c r="B47" t="s">
+        <v>231</v>
+      </c>
+      <c r="C47" t="s">
+        <v>224</v>
+      </c>
+      <c r="D47" t="s">
+        <v>58</v>
+      </c>
+      <c r="E47" t="s">
+        <v>200</v>
+      </c>
+      <c r="F47" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="4:4">
+      <c r="B48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C48" t="s">
+        <v>224</v>
+      </c>
+      <c r="D48" t="s">
+        <v>62</v>
+      </c>
+      <c r="E48" t="s">
+        <v>233</v>
+      </c>
+      <c r="F48" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="49" spans="4:4"/>
     <row r="50" spans="4:4"/>
     <row r="51" spans="4:4"/>

</xml_diff>